<commit_message>
Added fields to data dictionary and change to defnition of time since hypertension to account for missing values
</commit_message>
<xml_diff>
--- a/Outputs/DataDictionary.xlsx
+++ b/Outputs/DataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/uctvnjl_ucl_ac_uk/Documents/Post doc files/Repurposing/Repurposing-CCBs-in-SMI/Outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="342" documentId="8_{C3759D89-EB04-452C-869B-FC004333D791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{263AA131-75BE-49F6-8F76-AF3CC39F4934}"/>
+  <xr:revisionPtr revIDLastSave="357" documentId="8_{C3759D89-EB04-452C-869B-FC004333D791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{209A1ABB-B1F6-49BA-BAD5-29091DE7CC4E}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-5550" windowWidth="38640" windowHeight="21120" xr2:uid="{4219923E-13BB-43D4-AF54-161899A46BB0}"/>
+    <workbookView xWindow="-33960" yWindow="-1125" windowWidth="28800" windowHeight="15345" xr2:uid="{4219923E-13BB-43D4-AF54-161899A46BB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="290">
   <si>
     <t>patid</t>
   </si>
@@ -872,6 +872,24 @@
   </si>
   <si>
     <t>Variable name</t>
+  </si>
+  <si>
+    <t>CCBYear</t>
+  </si>
+  <si>
+    <t>Index year</t>
+  </si>
+  <si>
+    <t>AnyHyp</t>
+  </si>
+  <si>
+    <t>Any hypertension or high BP</t>
+  </si>
+  <si>
+    <t>Earliest of hypertension or high BP</t>
+  </si>
+  <si>
+    <t>TimeSinceAnyHyp</t>
   </si>
 </sst>
 </file>
@@ -1737,10 +1755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD21BADF-563A-40CF-A565-6F05AE59398E}">
-  <dimension ref="A1:D143"/>
+  <dimension ref="A1:D146"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2047,27 +2065,27 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>40</v>
+        <v>143</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>284</v>
       </c>
       <c r="C22" t="s">
-        <v>110</v>
+        <v>285</v>
       </c>
       <c r="D22" t="s">
-        <v>97</v>
+        <v>225</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D23" t="s">
         <v>97</v>
@@ -2075,13 +2093,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D24" t="s">
         <v>97</v>
@@ -2089,13 +2107,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D25" t="s">
         <v>97</v>
@@ -2103,13 +2121,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D26" t="s">
         <v>97</v>
@@ -2117,13 +2135,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D27" t="s">
         <v>97</v>
@@ -2131,13 +2149,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C28" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D28" t="s">
         <v>97</v>
@@ -2145,13 +2163,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D29" t="s">
         <v>97</v>
@@ -2159,13 +2177,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D30" t="s">
         <v>97</v>
@@ -2173,13 +2191,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D31" t="s">
         <v>97</v>
@@ -2187,13 +2205,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D32" t="s">
         <v>97</v>
@@ -2201,13 +2219,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C33" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D33" t="s">
         <v>97</v>
@@ -2215,13 +2233,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>95</v>
+        <v>144</v>
       </c>
       <c r="B34" t="s">
-        <v>79</v>
+        <v>286</v>
       </c>
       <c r="C34" t="s">
-        <v>122</v>
+        <v>287</v>
       </c>
       <c r="D34" t="s">
         <v>97</v>
@@ -2229,13 +2247,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C35" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D35" t="s">
         <v>97</v>
@@ -2243,13 +2261,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B36" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C36" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D36" t="s">
         <v>97</v>
@@ -2257,27 +2275,24 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>59</v>
+        <v>145</v>
       </c>
       <c r="B37" t="s">
-        <v>58</v>
+        <v>289</v>
       </c>
       <c r="C37" t="s">
-        <v>125</v>
-      </c>
-      <c r="D37" t="s">
-        <v>97</v>
+        <v>288</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>100</v>
+        <v>58</v>
       </c>
       <c r="B38" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="C38" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D38" t="s">
         <v>97</v>
@@ -2285,13 +2300,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>60</v>
+        <v>101</v>
       </c>
       <c r="B39" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="C39" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="D39" t="s">
         <v>97</v>
@@ -2299,13 +2314,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>98</v>
+        <v>59</v>
       </c>
       <c r="B40" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="C40" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="D40" t="s">
         <v>97</v>
@@ -2313,13 +2328,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>62</v>
+        <v>100</v>
       </c>
       <c r="B41" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="C41" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D41" t="s">
         <v>97</v>
@@ -2327,13 +2342,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B42" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C42" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="D42" t="s">
         <v>97</v>
@@ -2341,13 +2356,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>142</v>
+        <v>98</v>
       </c>
       <c r="B43" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="C43" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="D43" t="s">
         <v>97</v>
@@ -2355,13 +2370,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B44" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C44" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D44" t="s">
         <v>97</v>
@@ -2369,13 +2384,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B45" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C45" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D45" t="s">
         <v>97</v>
@@ -2383,13 +2398,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>67</v>
+        <v>142</v>
       </c>
       <c r="B46" t="s">
-        <v>66</v>
+        <v>93</v>
       </c>
       <c r="C46" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D46" t="s">
         <v>97</v>
@@ -2397,13 +2412,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B47" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C47" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D47" t="s">
         <v>97</v>
@@ -2411,13 +2426,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B48" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C48" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D48" t="s">
         <v>97</v>
@@ -2425,13 +2440,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B49" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C49" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D49" t="s">
         <v>97</v>
@@ -2439,13 +2454,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>107</v>
+        <v>68</v>
       </c>
       <c r="B50" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="C50" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D50" t="s">
         <v>97</v>
@@ -2453,13 +2468,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B51" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C51" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D51" t="s">
         <v>97</v>
@@ -2467,13 +2482,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>108</v>
+        <v>74</v>
       </c>
       <c r="B52" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="C52" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D52" t="s">
         <v>97</v>
@@ -2481,13 +2496,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="B53" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="C53" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D53" t="s">
         <v>97</v>
@@ -2495,13 +2510,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="B54" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="C54" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D54" t="s">
         <v>97</v>
@@ -2509,13 +2524,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="B55" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="C55" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D55" t="s">
         <v>97</v>
@@ -2523,13 +2538,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="B56" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C56" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D56" t="s">
         <v>97</v>
@@ -2537,13 +2552,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="B57" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C57" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D57" t="s">
         <v>97</v>
@@ -2551,13 +2566,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="B58" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="C58" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D58" t="s">
         <v>97</v>
@@ -2565,13 +2580,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="B59" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C59" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D59" t="s">
         <v>97</v>
@@ -2579,13 +2594,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>106</v>
+        <v>81</v>
       </c>
       <c r="B60" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="C60" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D60" t="s">
         <v>97</v>
@@ -2593,69 +2608,69 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>39</v>
+        <v>105</v>
       </c>
       <c r="B61" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C61" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D61" t="s">
-        <v>145</v>
+        <v>97</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="B62" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="C62" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D62" t="s">
-        <v>147</v>
+        <v>97</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>44</v>
+        <v>106</v>
       </c>
       <c r="B63" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
       <c r="C63" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="D63" t="s">
-        <v>147</v>
+        <v>97</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="B64" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="C64" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D64" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="B65" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="C65" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D65" t="s">
         <v>147</v>
@@ -2663,13 +2678,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>99</v>
+        <v>44</v>
       </c>
       <c r="B66" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="C66" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D66" t="s">
         <v>147</v>
@@ -2677,55 +2692,55 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>179</v>
+        <v>64</v>
       </c>
       <c r="C67" t="s">
-        <v>226</v>
+        <v>149</v>
       </c>
       <c r="D67" t="s">
-        <v>238</v>
+        <v>147</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>180</v>
+        <v>65</v>
       </c>
       <c r="C68" t="s">
-        <v>227</v>
+        <v>150</v>
       </c>
       <c r="D68" t="s">
-        <v>238</v>
+        <v>147</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="B69" t="s">
-        <v>181</v>
+        <v>83</v>
       </c>
       <c r="C69" t="s">
-        <v>228</v>
+        <v>151</v>
       </c>
       <c r="D69" t="s">
-        <v>238</v>
+        <v>147</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B70" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C70" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D70" t="s">
         <v>238</v>
@@ -2733,13 +2748,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B71" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C71" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D71" t="s">
         <v>238</v>
@@ -2747,13 +2762,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B72" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C72" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D72" t="s">
         <v>238</v>
@@ -2761,13 +2776,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B73" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C73" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D73" t="s">
         <v>238</v>
@@ -2775,13 +2790,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B74" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C74" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D74" t="s">
         <v>238</v>
@@ -2789,13 +2804,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B75" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C75" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D75" t="s">
         <v>238</v>
@@ -2803,13 +2818,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B76" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C76" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D76" t="s">
         <v>238</v>
@@ -2817,13 +2832,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B77" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C77" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D77" t="s">
         <v>238</v>
@@ -2831,13 +2846,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B78" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C78" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D78" t="s">
         <v>238</v>
@@ -2845,13 +2860,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="B79" t="s">
-        <v>243</v>
+        <v>189</v>
       </c>
       <c r="C79" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="D79" t="s">
         <v>238</v>
@@ -2859,13 +2874,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>115</v>
+        <v>91</v>
       </c>
       <c r="B80" t="s">
-        <v>244</v>
+        <v>190</v>
       </c>
       <c r="C80" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="D80" t="s">
         <v>238</v>
@@ -2873,13 +2888,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="B81" t="s">
-        <v>245</v>
+        <v>191</v>
       </c>
       <c r="C81" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="D81" t="s">
         <v>238</v>
@@ -2887,13 +2902,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B82" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C82" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D82" t="s">
         <v>238</v>
@@ -2901,13 +2916,13 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>138</v>
+        <v>115</v>
       </c>
       <c r="B83" t="s">
-        <v>219</v>
+        <v>244</v>
       </c>
       <c r="C83" t="s">
-        <v>239</v>
+        <v>248</v>
       </c>
       <c r="D83" t="s">
         <v>238</v>
@@ -2915,27 +2930,27 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="B84" t="s">
-        <v>217</v>
+        <v>245</v>
       </c>
       <c r="C84" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="D84" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="B85" t="s">
-        <v>215</v>
+        <v>246</v>
       </c>
       <c r="C85" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
       <c r="D85" t="s">
         <v>238</v>
@@ -2943,13 +2958,13 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B86" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="C86" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D86" t="s">
         <v>238</v>
@@ -2957,55 +2972,55 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="B87" t="s">
-        <v>198</v>
+        <v>217</v>
       </c>
       <c r="C87" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="D87" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="B88" t="s">
-        <v>199</v>
+        <v>215</v>
       </c>
       <c r="C88" t="s">
-        <v>257</v>
+        <v>241</v>
       </c>
       <c r="D88" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B89" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C89" t="s">
-        <v>261</v>
+        <v>242</v>
       </c>
       <c r="D89" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B90" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C90" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D90" t="s">
         <v>252</v>
@@ -3013,13 +3028,13 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B91" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C91" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D91" t="s">
         <v>252</v>
@@ -3027,13 +3042,13 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B92" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C92" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D92" t="s">
         <v>252</v>
@@ -3041,13 +3056,13 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B93" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C93" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D93" t="s">
         <v>252</v>
@@ -3055,13 +3070,13 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B94" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C94" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D94" t="s">
         <v>252</v>
@@ -3069,13 +3084,13 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B95" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C95" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D95" t="s">
         <v>252</v>
@@ -3083,13 +3098,13 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B96" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C96" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D96" t="s">
         <v>252</v>
@@ -3097,13 +3112,13 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B97" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C97" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D97" t="s">
         <v>252</v>
@@ -3111,13 +3126,13 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B98" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C98" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D98" t="s">
         <v>252</v>
@@ -3125,55 +3140,55 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="B99" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="C99" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="D99" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="B100" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="C100" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="D100" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>112</v>
+        <v>137</v>
       </c>
       <c r="B101" t="s">
-        <v>197</v>
+        <v>218</v>
       </c>
       <c r="C101" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="D101" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="B102" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="C102" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D102" t="s">
         <v>265</v>
@@ -3181,13 +3196,13 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="B103" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="C103" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D103" t="s">
         <v>265</v>
@@ -3195,13 +3210,13 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>139</v>
+        <v>112</v>
       </c>
       <c r="B104" t="s">
-        <v>220</v>
+        <v>197</v>
       </c>
       <c r="C104" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D104" t="s">
         <v>265</v>
@@ -3209,13 +3224,13 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B105" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C105" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D105" t="s">
         <v>265</v>
@@ -3223,13 +3238,13 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B106" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C106" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D106" t="s">
         <v>265</v>
@@ -3237,13 +3252,13 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B107" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C107" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D107" t="s">
         <v>265</v>
@@ -3251,13 +3266,13 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B108" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C108" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D108" t="s">
         <v>265</v>
@@ -3265,13 +3280,13 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B109" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C109" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D109" t="s">
         <v>265</v>
@@ -3279,13 +3294,13 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B110" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C110" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D110" t="s">
         <v>265</v>
@@ -3293,55 +3308,55 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>5</v>
+        <v>129</v>
       </c>
       <c r="B111" t="s">
-        <v>4</v>
+        <v>210</v>
       </c>
       <c r="C111" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="D111" t="s">
-        <v>153</v>
+        <v>265</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>6</v>
+        <v>130</v>
       </c>
       <c r="B112" t="s">
-        <v>5</v>
+        <v>211</v>
       </c>
       <c r="C112" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="D112" t="s">
-        <v>153</v>
+        <v>265</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>7</v>
+        <v>141</v>
       </c>
       <c r="B113" t="s">
-        <v>6</v>
+        <v>222</v>
       </c>
       <c r="C113" t="s">
-        <v>170</v>
+        <v>277</v>
       </c>
       <c r="D113" t="s">
-        <v>153</v>
+        <v>265</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B114" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C114" t="s">
-        <v>160</v>
+        <v>278</v>
       </c>
       <c r="D114" t="s">
         <v>153</v>
@@ -3349,13 +3364,13 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B115" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C115" t="s">
-        <v>161</v>
+        <v>279</v>
       </c>
       <c r="D115" t="s">
         <v>153</v>
@@ -3363,13 +3378,13 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B116" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C116" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="D116" t="s">
         <v>153</v>
@@ -3377,13 +3392,13 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B117" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C117" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D117" t="s">
         <v>153</v>
@@ -3391,10 +3406,10 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B118" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C118" t="s">
         <v>161</v>
@@ -3405,10 +3420,10 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B119" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C119" t="s">
         <v>161</v>
@@ -3419,10 +3434,10 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B120" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C120" t="s">
         <v>161</v>
@@ -3433,10 +3448,10 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B121" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C121" t="s">
         <v>161</v>
@@ -3447,13 +3462,13 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B122" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C122" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D122" t="s">
         <v>153</v>
@@ -3461,13 +3476,13 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B123" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C123" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="D123" t="s">
         <v>153</v>
@@ -3475,13 +3490,13 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B124" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C124" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="D124" t="s">
         <v>153</v>
@@ -3489,13 +3504,13 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B125" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C125" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="D125" t="s">
         <v>153</v>
@@ -3503,13 +3518,13 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B126" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C126" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D126" t="s">
         <v>153</v>
@@ -3517,13 +3532,13 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B127" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C127" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D127" t="s">
         <v>153</v>
@@ -3531,13 +3546,13 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B128" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C128" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D128" t="s">
         <v>153</v>
@@ -3545,13 +3560,13 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B129" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C129" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D129" t="s">
         <v>153</v>
@@ -3559,13 +3574,13 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B130" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C130" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="D130" t="s">
         <v>153</v>
@@ -3573,13 +3588,13 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B131" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C131" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="D131" t="s">
         <v>153</v>
@@ -3587,13 +3602,13 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="B132" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="C132" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D132" t="s">
         <v>153</v>
@@ -3601,13 +3616,13 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="B133" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="C133" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="D133" t="s">
         <v>153</v>
@@ -3615,13 +3630,13 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="B134" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="C134" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="D134" t="s">
         <v>153</v>
@@ -3629,13 +3644,13 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B135" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C135" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D135" t="s">
         <v>153</v>
@@ -3643,13 +3658,13 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B136" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C136" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D136" t="s">
         <v>153</v>
@@ -3657,13 +3672,13 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="B137" t="s">
-        <v>183</v>
+        <v>53</v>
       </c>
       <c r="C137" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D137" t="s">
         <v>153</v>
@@ -3671,13 +3686,13 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="B138" t="s">
-        <v>192</v>
+        <v>60</v>
       </c>
       <c r="C138" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="D138" t="s">
         <v>153</v>
@@ -3685,13 +3700,13 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="B139" t="s">
-        <v>193</v>
+        <v>62</v>
       </c>
       <c r="C139" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="D139" t="s">
         <v>153</v>
@@ -3699,13 +3714,13 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="B140" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="C140" t="s">
-        <v>251</v>
+        <v>171</v>
       </c>
       <c r="D140" t="s">
         <v>153</v>
@@ -3713,43 +3728,85 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="B141" t="s">
-        <v>35</v>
+        <v>192</v>
       </c>
       <c r="C141" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D141" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>37</v>
+        <v>94</v>
       </c>
       <c r="B142" t="s">
-        <v>36</v>
+        <v>193</v>
       </c>
       <c r="C142" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="D142" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143">
+        <v>110</v>
+      </c>
+      <c r="B143" t="s">
+        <v>195</v>
+      </c>
+      <c r="C143" t="s">
+        <v>251</v>
+      </c>
+      <c r="D143" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>36</v>
+      </c>
+      <c r="B144" t="s">
+        <v>35</v>
+      </c>
+      <c r="C144" t="s">
+        <v>172</v>
+      </c>
+      <c r="D144" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>37</v>
+      </c>
+      <c r="B145" t="s">
+        <v>36</v>
+      </c>
+      <c r="C145" t="s">
+        <v>174</v>
+      </c>
+      <c r="D145" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146">
         <v>38</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B146" t="s">
         <v>37</v>
       </c>
-      <c r="C143" t="s">
+      <c r="C146" t="s">
         <v>175</v>
       </c>
-      <c r="D143" t="s">
+      <c r="D146" t="s">
         <v>173</v>
       </c>
     </row>

</xml_diff>